<commit_message>
Save shop_data, leaderboard data , money, fix SFX
</commit_message>
<xml_diff>
--- a/Project2/map/map_stage3.xlsx
+++ b/Project2/map/map_stage3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JumpKing\Project2\map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0B2DA0-DB97-4BE6-A8B3-4C8939AB773A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7294FE-DC05-44CE-95FF-6B668F8C5592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{48E8A6F0-D45C-499F-B0E9-10C3D3B96F46}"/>
   </bookViews>
@@ -554,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7174F57D-9AE7-43AF-99BF-E0807E6314AC}">
   <dimension ref="A1:AO300"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
-      <selection activeCell="AN300" sqref="A1:AN300"/>
+    <sheetView tabSelected="1" topLeftCell="A263" zoomScale="56" workbookViewId="0">
+      <selection sqref="A1:AN300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -23555,38 +23555,38 @@
         <v>0</v>
       </c>
       <c r="T189" s="2">
+        <v>0</v>
+      </c>
+      <c r="U189" s="2">
+        <v>0</v>
+      </c>
+      <c r="V189" s="2">
+        <v>0</v>
+      </c>
+      <c r="W189" s="2">
+        <v>0</v>
+      </c>
+      <c r="X189" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y189" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z189" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA189" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB189" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC189" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD189" s="2">
         <v>93</v>
       </c>
-      <c r="U189" s="2">
-        <v>0</v>
-      </c>
-      <c r="V189" s="2">
-        <v>0</v>
-      </c>
-      <c r="W189" s="2">
-        <v>0</v>
-      </c>
-      <c r="X189" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y189" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z189" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA189" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB189" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC189" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD189" s="2">
-        <v>0</v>
-      </c>
       <c r="AE189" s="2">
         <v>0</v>
       </c>
@@ -23600,7 +23600,7 @@
         <v>0</v>
       </c>
       <c r="AI189" s="2">
-        <v>93</v>
+        <v>0</v>
       </c>
       <c r="AJ189" s="2">
         <v>0</v>
@@ -23799,7 +23799,7 @@
         <v>0</v>
       </c>
       <c r="T191" s="2">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="U191" s="2">
         <v>0</v>
@@ -25189,7 +25189,7 @@
         <v>0</v>
       </c>
       <c r="AJ202" s="2">
-        <v>93</v>
+        <v>0</v>
       </c>
       <c r="AK202" s="2">
         <v>0</v>
@@ -30676,7 +30676,7 @@
         <v>0</v>
       </c>
       <c r="AF247" s="2">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="AG247" s="2">
         <v>0</v>
@@ -30685,7 +30685,7 @@
         <v>0</v>
       </c>
       <c r="AI247" s="2">
-        <v>93</v>
+        <v>0</v>
       </c>
       <c r="AJ247" s="2">
         <v>0</v>
@@ -37175,7 +37175,7 @@
       <formula>A1048563=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:AN106 A107:X117 Y107:AN118 A118:A124 B119:AN124 A125:AN300 AO218:AO226 B2:AM217">
+  <conditionalFormatting sqref="A1:AN106 B2:AM217 A107:X117 Y107:AN118 A118:A124 B119:AN124 A125:AN300 AO218:AO226">
     <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
       <formula>50</formula>
     </cfRule>
@@ -37189,7 +37189,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AO218:AO226 A1:AN300">
+  <conditionalFormatting sqref="A1:AN300 AO218:AO226">
     <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>60</formula>
     </cfRule>

</xml_diff>